<commit_message>
Update SA templates with new field
</commit_message>
<xml_diff>
--- a/DCR_MODS_templates/SA-MODS-template-v3.xlsx
+++ b/DCR_MODS_templates/SA-MODS-template-v3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Desktop\dcr_mods_templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goslen\Git\Metadata-Miscellany\DCR_MODS_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF985ED9-2973-476D-B10E-5AC9FC576A41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED08E392-5EA1-4951-B6A0-3D7A0E74BC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30AE1F1C-9D6D-4975-B041-019DDB28DD50}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Contributor (Participant) Name</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>&lt;/mods:mods&gt;&lt;/update&gt;&lt;/object&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;mods:description&gt;Ethnic or Racial Identity: </t>
+  </si>
+  <si>
+    <t>Ethnic or Racial Identity</t>
   </si>
 </sst>
 </file>
@@ -569,30 +575,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589D00E9-24EF-4C42-B836-025FE26EDFD9}">
-  <dimension ref="A1:BJ1"/>
+  <dimension ref="A1:BM1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" customWidth="1"/>
-    <col min="33" max="33" width="17.5703125" customWidth="1"/>
-    <col min="36" max="36" width="30.85546875" customWidth="1"/>
-    <col min="48" max="48" width="12.5703125" style="5" customWidth="1"/>
-    <col min="54" max="54" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="24.88671875" customWidth="1"/>
+    <col min="14" max="14" width="10" customWidth="1"/>
+    <col min="17" max="17" width="15.88671875" customWidth="1"/>
+    <col min="20" max="20" width="24.88671875" customWidth="1"/>
+    <col min="24" max="24" width="9.109375" customWidth="1"/>
+    <col min="27" max="27" width="18.5546875" customWidth="1"/>
+    <col min="33" max="33" width="11.33203125" customWidth="1"/>
+    <col min="36" max="36" width="17.5546875" customWidth="1"/>
+    <col min="39" max="39" width="30.88671875" customWidth="1"/>
+    <col min="51" max="51" width="12.5546875" style="5" customWidth="1"/>
+    <col min="57" max="57" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:65" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -621,162 +627,171 @@
         <v>22</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="L1" t="s">
         <v>22</v>
       </c>
       <c r="M1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O1" t="s">
         <v>22</v>
       </c>
       <c r="P1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R1" t="s">
         <v>22</v>
       </c>
       <c r="S1" t="s">
+        <v>25</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" t="s">
         <v>26</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>27</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>28</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>34</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>35</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="AK1" t="s">
         <v>36</v>
       </c>
       <c r="AL1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AN1" t="s">
         <v>36</v>
       </c>
       <c r="AO1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR1" t="s">
         <v>37</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>43</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>44</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>45</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>46</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>47</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BI1" t="s">
         <v>36</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
         <v>48</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BM1" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>